<commit_message>
using just the number of objects for calculating noise.
</commit_message>
<xml_diff>
--- a/model/SMsheet.xlsx
+++ b/model/SMsheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="3000" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="2380" yWindow="560" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>=========  Results  ===========</t>
   </si>
@@ -120,31 +120,19 @@
     <t>&gt; (run-analysis 100)</t>
   </si>
   <si>
-    <t>noise = Math.min(base + scale * Math.exp(-activation), 8 )</t>
-  </si>
-  <si>
-    <t>base = 0</t>
-  </si>
-  <si>
-    <t>scale = .1</t>
-  </si>
-  <si>
     <t xml:space="preserve">    :ans 0.5</t>
   </si>
   <si>
-    <t xml:space="preserve">    :rt -0.5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    :bll 0.8</t>
-  </si>
-  <si>
-    <t>double base = .0;</t>
-  </si>
-  <si>
-    <t>double scale = .1;</t>
-  </si>
-  <si>
     <t>double noise = Math.min(base + scale * Math.exp(-activation) + numberOfObjects/200.0 , 0.1 );</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    :bll 0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    :rt -0.5  </t>
+  </si>
+  <si>
+    <t>double noise = Math.pow(numberOfObjects/2.0, 2) / 100.0 ;</t>
   </si>
 </sst>
 </file>
@@ -199,8 +187,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -268,7 +258,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -299,6 +289,7 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -329,6 +320,7 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,10 +366,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>50.7</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.1</c:v>
+                  <c:v>73.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -430,13 +422,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>55.3</c:v>
+                  <c:v>58.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.5</c:v>
+                  <c:v>82.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>94.0</c:v>
+                  <c:v>100.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -490,16 +482,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>58.8</c:v>
+                  <c:v>64.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.1</c:v>
+                  <c:v>85.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95.1</c:v>
+                  <c:v>102.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>112.8</c:v>
+                  <c:v>115.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,19 +548,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>61.8</c:v>
+                  <c:v>71.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>81.8</c:v>
+                  <c:v>89.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.4</c:v>
+                  <c:v>104.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>115.5</c:v>
+                  <c:v>119.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>131.5</c:v>
+                  <c:v>123.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -620,11 +612,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081791176"/>
-        <c:axId val="2081796648"/>
+        <c:axId val="2125416776"/>
+        <c:axId val="2126631288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081791176"/>
+        <c:axId val="2125416776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -652,7 +644,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081796648"/>
+        <c:crossAx val="2126631288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -660,7 +652,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081796648"/>
+        <c:axId val="2126631288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -690,7 +682,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081791176"/>
+        <c:crossAx val="2125416776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -755,10 +747,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>48.7</c:v>
+                  <c:v>45.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.0</c:v>
+                  <c:v>70.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -811,13 +803,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>49.2</c:v>
+                  <c:v>58.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.9</c:v>
+                  <c:v>79.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.4</c:v>
+                  <c:v>95.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -871,16 +863,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>49.7</c:v>
+                  <c:v>66.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>75.0</c:v>
+                  <c:v>87.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.3</c:v>
+                  <c:v>102.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>117.2</c:v>
+                  <c:v>112.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,19 +929,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>51.4</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.5</c:v>
+                  <c:v>94.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.5</c:v>
+                  <c:v>114.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>115.5</c:v>
+                  <c:v>121.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>133.7</c:v>
+                  <c:v>129.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1001,11 +993,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081879016"/>
-        <c:axId val="2081884488"/>
+        <c:axId val="2126718952"/>
+        <c:axId val="2126724424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081879016"/>
+        <c:axId val="2126718952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,7 +1025,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081884488"/>
+        <c:crossAx val="2126724424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1041,7 +1033,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081884488"/>
+        <c:axId val="2126724424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1063,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081879016"/>
+        <c:crossAx val="2126718952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1103,15 +1095,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
+      <xdr:colOff>660400</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>241300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1489,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1659,130 +1651,130 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>47.3</v>
+        <v>50.1</v>
       </c>
       <c r="C10">
-        <v>54.1</v>
+        <v>54.9</v>
       </c>
       <c r="D10">
-        <v>50.6</v>
+        <v>60</v>
       </c>
       <c r="E10">
-        <v>65.3</v>
+        <v>69</v>
       </c>
       <c r="F10">
-        <v>77</v>
+        <v>73.5</v>
       </c>
       <c r="G10">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H10">
         <v>54.5</v>
       </c>
       <c r="I10">
-        <v>51</v>
+        <v>57.6</v>
       </c>
       <c r="J10">
-        <v>60.4</v>
+        <v>62.4</v>
       </c>
       <c r="K10">
-        <v>72.599999999999994</v>
+        <v>80.2</v>
       </c>
       <c r="L10">
-        <v>71.5</v>
+        <v>82.8</v>
       </c>
       <c r="M10">
-        <v>79.3</v>
+        <v>85.5</v>
       </c>
       <c r="N10">
-        <v>84.8</v>
+        <v>92</v>
       </c>
       <c r="O10">
-        <v>95.2</v>
+        <v>106.9</v>
       </c>
       <c r="P10">
+        <v>101.5</v>
+      </c>
+      <c r="Q10">
+        <v>58.4</v>
+      </c>
+      <c r="R10">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="S10">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="T10">
+        <v>78.8</v>
+      </c>
+      <c r="U10">
+        <v>90.3</v>
+      </c>
+      <c r="V10">
+        <v>87.2</v>
+      </c>
+      <c r="W10">
+        <v>97</v>
+      </c>
+      <c r="X10">
+        <v>104.5</v>
+      </c>
+      <c r="Y10">
+        <v>105.8</v>
+      </c>
+      <c r="Z10">
+        <v>115</v>
+      </c>
+      <c r="AA10">
+        <v>112.1</v>
+      </c>
+      <c r="AB10">
+        <v>119.3</v>
+      </c>
+      <c r="AC10">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="AD10">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="AE10">
+        <v>79</v>
+      </c>
+      <c r="AF10">
+        <v>87.8</v>
+      </c>
+      <c r="AG10">
+        <v>89.9</v>
+      </c>
+      <c r="AH10">
+        <v>89.2</v>
+      </c>
+      <c r="AI10">
+        <v>105.4</v>
+      </c>
+      <c r="AJ10">
         <v>101.9</v>
       </c>
-      <c r="Q10">
-        <v>57.7</v>
-      </c>
-      <c r="R10">
-        <v>55.2</v>
-      </c>
-      <c r="S10">
-        <v>63.6</v>
-      </c>
-      <c r="T10">
-        <v>77.099999999999994</v>
-      </c>
-      <c r="U10">
-        <v>82</v>
-      </c>
-      <c r="V10">
-        <v>81.099999999999994</v>
-      </c>
-      <c r="W10">
-        <v>87.4</v>
-      </c>
-      <c r="X10">
-        <v>94</v>
-      </c>
-      <c r="Y10">
-        <v>103.8</v>
-      </c>
-      <c r="Z10">
-        <v>104.5</v>
-      </c>
-      <c r="AA10">
-        <v>117.9</v>
-      </c>
-      <c r="AB10">
-        <v>116.2</v>
-      </c>
-      <c r="AC10">
-        <v>59.4</v>
-      </c>
-      <c r="AD10">
-        <v>58.9</v>
-      </c>
-      <c r="AE10">
-        <v>67.099999999999994</v>
-      </c>
-      <c r="AF10">
-        <v>79.3</v>
-      </c>
-      <c r="AG10">
-        <v>75.400000000000006</v>
-      </c>
-      <c r="AH10">
-        <v>90.7</v>
-      </c>
-      <c r="AI10">
-        <v>96.5</v>
-      </c>
-      <c r="AJ10">
-        <v>104.3</v>
-      </c>
       <c r="AK10">
-        <v>100.5</v>
+        <v>106.9</v>
       </c>
       <c r="AL10">
-        <v>108.5</v>
+        <v>118.7</v>
       </c>
       <c r="AM10">
-        <v>117</v>
+        <v>114.6</v>
       </c>
       <c r="AN10">
-        <v>121</v>
+        <v>126.5</v>
       </c>
       <c r="AO10">
-        <v>129.5</v>
+        <v>120.4</v>
       </c>
       <c r="AP10">
-        <v>130.80000000000001</v>
+        <v>127.6</v>
       </c>
       <c r="AQ10">
-        <v>134.1</v>
+        <v>122.9</v>
       </c>
     </row>
     <row r="12" spans="1:43">
@@ -1926,130 +1918,130 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="C14">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="D14">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="F14">
+        <v>2.1</v>
+      </c>
+      <c r="G14">
+        <v>2.1</v>
+      </c>
+      <c r="H14">
         <v>1.9</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>1.9</v>
       </c>
-      <c r="H14">
-        <v>1.6</v>
-      </c>
-      <c r="I14">
-        <v>1.6</v>
-      </c>
       <c r="J14">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="K14">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="L14">
-        <v>1.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q14">
         <v>1.9</v>
       </c>
-      <c r="N14">
+      <c r="R14">
         <v>2</v>
       </c>
-      <c r="O14">
+      <c r="S14">
         <v>2</v>
       </c>
-      <c r="P14">
-        <v>2.1</v>
-      </c>
-      <c r="Q14">
-        <v>1.6</v>
-      </c>
-      <c r="R14">
-        <v>1.6</v>
-      </c>
-      <c r="S14">
-        <v>1.6</v>
-      </c>
       <c r="T14">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="U14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="W14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Y14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA14">
+        <v>2.4</v>
+      </c>
+      <c r="AB14">
+        <v>2.4</v>
+      </c>
+      <c r="AC14">
         <v>1.9</v>
       </c>
-      <c r="V14">
-        <v>1.9</v>
-      </c>
-      <c r="W14">
+      <c r="AD14">
         <v>2</v>
       </c>
-      <c r="X14">
+      <c r="AE14">
         <v>2</v>
       </c>
-      <c r="Y14">
-        <v>2.1</v>
-      </c>
-      <c r="Z14">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AA14">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AB14">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AC14">
-        <v>1.6</v>
-      </c>
-      <c r="AD14">
-        <v>1.6</v>
-      </c>
-      <c r="AE14">
-        <v>1.7</v>
-      </c>
       <c r="AF14">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="AG14">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AH14">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AI14">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AJ14">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AK14">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AL14">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AM14">
         <v>2.2999999999999998</v>
       </c>
       <c r="AN14">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="AO14">
         <v>2.2999999999999998</v>
       </c>
       <c r="AP14">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="AQ14">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -2057,7 +2049,7 @@
         <v>30</v>
       </c>
       <c r="B17">
-        <v>12.23</v>
+        <v>10.37</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -2065,7 +2057,7 @@
         <v>31</v>
       </c>
       <c r="B18">
-        <v>0.41</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -2182,46 +2174,46 @@
         <v>7</v>
       </c>
       <c r="B26">
-        <v>50.7</v>
+        <v>55</v>
       </c>
       <c r="C26">
-        <v>74.099999999999994</v>
+        <v>73.8</v>
       </c>
       <c r="D26">
-        <v>55.3</v>
+        <v>58.2</v>
       </c>
       <c r="E26">
-        <v>74.5</v>
+        <v>82.8</v>
       </c>
       <c r="F26">
-        <v>94</v>
+        <v>100.1</v>
       </c>
       <c r="G26">
-        <v>58.8</v>
+        <v>64.5</v>
       </c>
       <c r="H26">
-        <v>80.099999999999994</v>
+        <v>85.4</v>
       </c>
       <c r="I26">
-        <v>95.1</v>
+        <v>102.4</v>
       </c>
       <c r="J26">
-        <v>112.8</v>
+        <v>115.5</v>
       </c>
       <c r="K26">
-        <v>61.8</v>
+        <v>71.3</v>
       </c>
       <c r="L26">
-        <v>81.8</v>
+        <v>89</v>
       </c>
       <c r="M26">
-        <v>100.4</v>
+        <v>104.7</v>
       </c>
       <c r="N26">
-        <v>115.5</v>
+        <v>119.9</v>
       </c>
       <c r="O26">
-        <v>131.5</v>
+        <v>123.6</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -2276,46 +2268,46 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="C28">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="D28">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="E28">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="F28">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G28">
+        <v>1.9</v>
+      </c>
+      <c r="H28">
+        <v>2.1</v>
+      </c>
+      <c r="I28">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J28">
+        <v>2.4</v>
+      </c>
+      <c r="K28">
         <v>2</v>
       </c>
-      <c r="G28">
-        <v>1.6</v>
-      </c>
-      <c r="H28">
-        <v>1.9</v>
-      </c>
-      <c r="I28">
-        <v>2.1</v>
-      </c>
-      <c r="J28">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K28">
-        <v>1.6</v>
-      </c>
       <c r="L28">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M28">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N28">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="O28">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -2323,7 +2315,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>11.37</v>
+        <v>9.33</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2331,50 +2323,35 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="23">
       <c r="A45" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="C46" t="s">
-        <v>34</v>
-      </c>
+      <c r="C45" s="2"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="C47" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
@@ -2527,130 +2504,130 @@
         <v>9</v>
       </c>
       <c r="B54">
-        <v>41.2</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="C54">
-        <v>51</v>
+        <v>46.3</v>
       </c>
       <c r="D54">
-        <v>53.8</v>
+        <v>51.2</v>
       </c>
       <c r="E54">
-        <v>63.8</v>
+        <v>62.1</v>
       </c>
       <c r="F54">
-        <v>77.2</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="G54">
-        <v>78.099999999999994</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="H54">
-        <v>45.8</v>
+        <v>46.7</v>
       </c>
       <c r="I54">
-        <v>44.3</v>
+        <v>60.3</v>
       </c>
       <c r="J54">
-        <v>57.5</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="K54">
-        <v>68.8</v>
+        <v>70.599999999999994</v>
       </c>
       <c r="L54">
-        <v>70.900000000000006</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="M54">
-        <v>81.8</v>
+        <v>84.7</v>
       </c>
       <c r="N54">
+        <v>89.9</v>
+      </c>
+      <c r="O54">
+        <v>95.2</v>
+      </c>
+      <c r="P54">
+        <v>100.9</v>
+      </c>
+      <c r="Q54">
+        <v>55.5</v>
+      </c>
+      <c r="R54">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="S54">
+        <v>70.3</v>
+      </c>
+      <c r="T54">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="U54">
+        <v>87.6</v>
+      </c>
+      <c r="V54">
+        <v>94.6</v>
+      </c>
+      <c r="W54">
+        <v>103</v>
+      </c>
+      <c r="X54">
+        <v>105.2</v>
+      </c>
+      <c r="Y54">
+        <v>100.6</v>
+      </c>
+      <c r="Z54">
+        <v>110.5</v>
+      </c>
+      <c r="AA54">
+        <v>110.9</v>
+      </c>
+      <c r="AB54">
+        <v>116.2</v>
+      </c>
+      <c r="AC54">
+        <v>73</v>
+      </c>
+      <c r="AD54">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="AE54">
+        <v>84.4</v>
+      </c>
+      <c r="AF54">
+        <v>91.8</v>
+      </c>
+      <c r="AG54">
         <v>94.4</v>
       </c>
-      <c r="O54">
-        <v>99.8</v>
-      </c>
-      <c r="P54">
-        <v>101</v>
-      </c>
-      <c r="Q54">
-        <v>43.8</v>
-      </c>
-      <c r="R54">
-        <v>51.5</v>
-      </c>
-      <c r="S54">
-        <v>53.8</v>
-      </c>
-      <c r="T54">
-        <v>74.3</v>
-      </c>
-      <c r="U54">
-        <v>76.7</v>
-      </c>
-      <c r="V54">
-        <v>74.2</v>
-      </c>
-      <c r="W54">
-        <v>96.4</v>
-      </c>
-      <c r="X54">
-        <v>100.4</v>
-      </c>
-      <c r="Y54">
+      <c r="AH54">
         <v>98.1</v>
       </c>
-      <c r="Z54">
-        <v>117.5</v>
-      </c>
-      <c r="AA54">
-        <v>112.1</v>
-      </c>
-      <c r="AB54">
-        <v>121.8</v>
-      </c>
-      <c r="AC54">
-        <v>48.7</v>
-      </c>
-      <c r="AD54">
-        <v>50.7</v>
-      </c>
-      <c r="AE54">
-        <v>54.7</v>
-      </c>
-      <c r="AF54">
-        <v>81.400000000000006</v>
-      </c>
-      <c r="AG54">
-        <v>75.2</v>
-      </c>
-      <c r="AH54">
-        <v>79</v>
-      </c>
       <c r="AI54">
-        <v>95.3</v>
+        <v>114.4</v>
       </c>
       <c r="AJ54">
-        <v>101.5</v>
+        <v>108.1</v>
       </c>
       <c r="AK54">
-        <v>104.8</v>
+        <v>120</v>
       </c>
       <c r="AL54">
-        <v>111.7</v>
+        <v>124</v>
       </c>
       <c r="AM54">
-        <v>118.9</v>
+        <v>119</v>
       </c>
       <c r="AN54">
-        <v>115.8</v>
+        <v>121.5</v>
       </c>
       <c r="AO54">
-        <v>132.69999999999999</v>
+        <v>127.8</v>
       </c>
       <c r="AP54">
-        <v>136.19999999999999</v>
+        <v>129.69999999999999</v>
       </c>
       <c r="AQ54">
-        <v>132.19999999999999</v>
+        <v>131.30000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:43">
@@ -2794,130 +2771,130 @@
         <v>11</v>
       </c>
       <c r="B58">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="C58">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="D58">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="E58">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="F58">
+        <v>2.1</v>
+      </c>
+      <c r="G58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H58">
         <v>1.9</v>
       </c>
-      <c r="G58">
+      <c r="I58">
         <v>1.9</v>
       </c>
-      <c r="H58">
-        <v>1.5</v>
-      </c>
-      <c r="I58">
-        <v>1.6</v>
-      </c>
       <c r="J58">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="K58">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="L58">
-        <v>1.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P58">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q58">
         <v>1.9</v>
       </c>
-      <c r="N58">
+      <c r="R58">
         <v>2</v>
       </c>
-      <c r="O58">
-        <v>2.1</v>
-      </c>
-      <c r="P58">
-        <v>2.1</v>
-      </c>
-      <c r="Q58">
-        <v>1.5</v>
-      </c>
-      <c r="R58">
-        <v>1.6</v>
-      </c>
       <c r="S58">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="T58">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="U58">
+        <v>2.1</v>
+      </c>
+      <c r="V58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="W58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X58">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Y58">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z58">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA58">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AB58">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AC58">
         <v>1.9</v>
       </c>
-      <c r="V58">
-        <v>1.9</v>
-      </c>
-      <c r="W58">
-        <v>2.1</v>
-      </c>
-      <c r="X58">
-        <v>2.1</v>
-      </c>
-      <c r="Y58">
-        <v>2.1</v>
-      </c>
-      <c r="Z58">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AA58">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AB58">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="AC58">
-        <v>1.6</v>
-      </c>
       <c r="AD58">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="AE58">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="AF58">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="AG58">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="AH58">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AI58">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AJ58">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AK58">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AL58">
-        <v>2.2000000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="AM58">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AN58">
-        <v>2.2000000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="AO58">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="AP58">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="AQ58">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="61" spans="1:43">
@@ -2925,7 +2902,7 @@
         <v>30</v>
       </c>
       <c r="B61">
-        <v>14.6</v>
+        <v>7.88</v>
       </c>
     </row>
     <row r="62" spans="1:43">
@@ -2933,7 +2910,7 @@
         <v>31</v>
       </c>
       <c r="B62">
-        <v>0.41</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="64" spans="1:43">
@@ -3050,46 +3027,46 @@
         <v>7</v>
       </c>
       <c r="B70">
-        <v>48.7</v>
+        <v>45.4</v>
       </c>
       <c r="C70">
-        <v>73</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="D70">
-        <v>49.2</v>
+        <v>58.4</v>
       </c>
       <c r="E70">
-        <v>73.900000000000006</v>
+        <v>79</v>
       </c>
       <c r="F70">
-        <v>98.4</v>
+        <v>95.3</v>
       </c>
       <c r="G70">
-        <v>49.7</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="H70">
-        <v>75</v>
+        <v>87.8</v>
       </c>
       <c r="I70">
-        <v>98.3</v>
+        <v>102.9</v>
       </c>
       <c r="J70">
-        <v>117.2</v>
+        <v>112.6</v>
       </c>
       <c r="K70">
-        <v>51.4</v>
+        <v>79.5</v>
       </c>
       <c r="L70">
-        <v>78.5</v>
+        <v>94.8</v>
       </c>
       <c r="M70">
-        <v>100.5</v>
+        <v>114.2</v>
       </c>
       <c r="N70">
-        <v>115.5</v>
+        <v>121.5</v>
       </c>
       <c r="O70">
-        <v>133.69999999999999</v>
+        <v>129.6</v>
       </c>
     </row>
     <row r="71" spans="1:15">
@@ -3144,46 +3121,46 @@
         <v>29</v>
       </c>
       <c r="B72">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="C72">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="D72">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="E72">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="F72">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G72">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="H72">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="I72">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="J72">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K72">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="L72">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="M72">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N72">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="O72">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="75" spans="1:15">
@@ -3191,7 +3168,7 @@
         <v>30</v>
       </c>
       <c r="B75">
-        <v>13.94</v>
+        <v>6.21</v>
       </c>
     </row>
     <row r="76" spans="1:15">
@@ -3199,26 +3176,30 @@
         <v>31</v>
       </c>
       <c r="B76">
-        <v>0.41</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="79" spans="1:15">
       <c r="A79" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="80" spans="1:15">
       <c r="A80" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="C80" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>